<commit_message>
done with new structure
</commit_message>
<xml_diff>
--- a/tests/test_project_data/experiment_information.xlsx
+++ b/tests/test_project_data/experiment_information.xlsx
@@ -434,55 +434,60 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>groups</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>experiment</t>
+          <t>independant_variables</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>groups</t>
+          <t>paired</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>independant_variables</t>
+          <t>parametric</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>paired</t>
+          <t>label</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>parametric</t>
+          <t>control_group_id</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1, 5, 3, 4</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TCB2, MDL</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>agonist antagonist</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1, 5, 3, 4</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>TCB2, MDL</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
+      <c r="F2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>